<commit_message>
adding sentence id / smaller changes to sentences
</commit_message>
<xml_diff>
--- a/wahlprogrammquiz/sample41_edited.xlsx
+++ b/wahlprogrammquiz/sample41_edited.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15615"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="670">
   <si>
     <t>partyabbrev</t>
   </si>
@@ -1344,9 +1344,6 @@
     <t>In der digitalen Welt gilt es, den Zugang zu Informationen zu verteidigen. Wir fordern, dass Daten und Informationen, die von Regierungen mit öffentlichen Geldern gesammelt und erstellt wurden, allen Menschen frei zugänglich und nutzbar gemacht werden. Die so geschaffenen "offenen Daten" (Open Data) können ein Beitrag zu einer Öffnung und Demokratisierung von Verwaltung sein. Dabei muss selbstverständlich der Datenschutz berücksichtigt werden. Wir wollen, dass die Nutzerinnen und Nutzer sich im Internet frei informieren, weiterbilden, äußern und partizipieren können. Wir wollen die offene Architektur des Netzes bewahren und so sein Potenzial für Innovation und Entwicklung fördern. Dazu gehört für uns, die Netzneutralität abzusichern. Um Netzneutralität und gute Versorgung sicher zu stellen, sollen die Telekommunikationsnetze in öffentliches und gemeinwirtschaftliches Eigentum überführt werden.Die Glasfaserinfrastruktur wollen wir rasch und flächendeckend ausbauen (vgl. Kapitel VI "In die Zukunft investieren"). Wir unterstützen Open Content-Lizenzen, die sich an Grundwerten von Offenheit und Teilhabe orientieren.</t>
   </si>
   <si>
-    <t>- Kinder brauchen Erwachsene, die sich liebevoll und verbindlich um sie kümmern. Eltern und Sorgeberechtigte sind nicht unbedingt dieselben Personen. Wir setzen uns dafür ein, dass auch (bis zu) vier Personen Eltern für ein Kind sein können, also in Co-Elternschaft das gemeinsame Sorgerecht Neben den Pflichten betrifft das auch Rechte wie Kinderfreibeträge und Renten ansprüche.</t>
-  </si>
-  <si>
     <t>DIE LINKE wendet sich dagegen, EU-Beitrittsverhandlungen mit autoritären Regimen wie im Falle der Türkei zu intensivieren. Wir treten für eine radikale Wende der deutschen und europäischen Türkeipolitik ein. Wir stehen an der Seite der Demokraten in der Türkei und fordern einen sofortigen Stopp der Rüstungsexporte und der Lieferungen von Rüstungsfabriken. DIE LINKE setzt sich für die Freilassung der politischen Gefangenen in der Türkei ein und steht allen Versuchen, dem türkischen Staatspräsidenten Erdogan unter die Arme zu greifen, wie mit einer Erweiterung der Zollunion, entgegen.</t>
   </si>
   <si>
@@ -2023,6 +2020,15 @@
   </si>
   <si>
     <t>Wir wollen die Unterbringung von Geflüchteten in Massenunterkünften beenden und dezentral organisieren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wir setzen uns dafür ein, dass auch (bis zu) vier Personen Eltern für ein Kind sein können, also in Co-Elternschaft das gemeinsame Sorgerecht innehaben. </t>
+  </si>
+  <si>
+    <t>Neben den Pflichten betrifft das auch Rechte wie Kinderfreibeträge und Rentenansprüche.</t>
+  </si>
+  <si>
+    <t>- Kinder brauchen Erwachsene, die sich liebevoll und verbindlich um sie kümmern. Eltern und Sorgeberechtigte sind nicht unbedingt dieselben Personen. Wir setzen uns dafür ein, dass auch (bis zu) vier Personen Eltern für ein Kind sein können, also in Co-Elternschaft das gemeinsame Sorgerecht innehaben. Neben den Pflichten betrifft das auch Rechte wie Kinderfreibeträge und Rentenansprüche.</t>
   </si>
 </sst>
 </file>
@@ -2058,14 +2064,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2393,18 +2405,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="136.33203125" customWidth="1"/>
+    <col min="3" max="3" width="136.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2458,7 +2470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2505,16 +2517,16 @@
         <v>338</v>
       </c>
       <c r="P2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="R2" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2561,16 +2573,16 @@
         <v>339</v>
       </c>
       <c r="P3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="Q3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="R3" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2617,16 +2629,16 @@
         <v>340</v>
       </c>
       <c r="P4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="Q4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R4" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2673,16 +2685,16 @@
         <v>341</v>
       </c>
       <c r="P5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R5" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2729,16 +2741,16 @@
         <v>27</v>
       </c>
       <c r="P6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R6" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2785,16 +2797,16 @@
         <v>342</v>
       </c>
       <c r="P7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="Q7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R7" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2841,16 +2853,16 @@
         <v>29</v>
       </c>
       <c r="P8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R8" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2897,16 +2909,16 @@
         <v>30</v>
       </c>
       <c r="P9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R9" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2953,16 +2965,16 @@
         <v>31</v>
       </c>
       <c r="P10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R10" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3009,16 +3021,16 @@
         <v>343</v>
       </c>
       <c r="P11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="R11" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3065,16 +3077,16 @@
         <v>33</v>
       </c>
       <c r="P12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R12" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3121,16 +3133,16 @@
         <v>344</v>
       </c>
       <c r="P13" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q13" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="R13" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3177,16 +3189,16 @@
         <v>35</v>
       </c>
       <c r="P14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R14" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3233,16 +3245,16 @@
         <v>345</v>
       </c>
       <c r="P15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q15" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="R15" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3289,16 +3301,16 @@
         <v>37</v>
       </c>
       <c r="P16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R16" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3345,16 +3357,16 @@
         <v>38</v>
       </c>
       <c r="P17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R17" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -3401,16 +3413,16 @@
         <v>346</v>
       </c>
       <c r="P18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="Q18" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="R18" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -3457,16 +3469,16 @@
         <v>347</v>
       </c>
       <c r="P19" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="Q19" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R19" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -3513,16 +3525,16 @@
         <v>348</v>
       </c>
       <c r="P20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Q20" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R20" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -3569,16 +3581,16 @@
         <v>42</v>
       </c>
       <c r="P21" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q21" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R21" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -3625,16 +3637,16 @@
         <v>349</v>
       </c>
       <c r="P22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="Q22" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="R22" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -3681,16 +3693,16 @@
         <v>44</v>
       </c>
       <c r="P23" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q23" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R23" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3737,16 +3749,16 @@
         <v>45</v>
       </c>
       <c r="P24" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q24" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R24" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -3793,16 +3805,16 @@
         <v>350</v>
       </c>
       <c r="P25" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q25" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="R25" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3849,16 +3861,16 @@
         <v>351</v>
       </c>
       <c r="P26" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q26" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="R26" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -3905,16 +3917,16 @@
         <v>48</v>
       </c>
       <c r="P27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R27" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -3961,16 +3973,16 @@
         <v>352</v>
       </c>
       <c r="P28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="Q28" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="R28" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -4017,16 +4029,16 @@
         <v>353</v>
       </c>
       <c r="P29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q29" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="R29" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -4073,16 +4085,16 @@
         <v>354</v>
       </c>
       <c r="P30" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Q30" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="R30" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -4129,16 +4141,16 @@
         <v>355</v>
       </c>
       <c r="P31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="Q31" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="R31" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -4185,16 +4197,16 @@
         <v>356</v>
       </c>
       <c r="P32" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="R32" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -4241,16 +4253,16 @@
         <v>54</v>
       </c>
       <c r="P33" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q33" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R33" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -4297,16 +4309,16 @@
         <v>357</v>
       </c>
       <c r="P34" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Q34" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="R34" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -4353,16 +4365,16 @@
         <v>358</v>
       </c>
       <c r="P35" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q35" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="R35" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -4409,16 +4421,16 @@
         <v>359</v>
       </c>
       <c r="P36" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="Q36" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="R36" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -4465,16 +4477,16 @@
         <v>360</v>
       </c>
       <c r="P37" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q37" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="R37" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -4521,16 +4533,16 @@
         <v>361</v>
       </c>
       <c r="P38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q38" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="R38" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -4577,16 +4589,16 @@
         <v>362</v>
       </c>
       <c r="P39" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q39" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="R39" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -4633,16 +4645,16 @@
         <v>363</v>
       </c>
       <c r="P40" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q40" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="R40" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -4689,16 +4701,16 @@
         <v>364</v>
       </c>
       <c r="P41" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q41" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="R41" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -4745,16 +4757,16 @@
         <v>362</v>
       </c>
       <c r="P42" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Q42" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="R42" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -4801,16 +4813,16 @@
         <v>365</v>
       </c>
       <c r="P43" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q43" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R43" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -4857,16 +4869,16 @@
         <v>366</v>
       </c>
       <c r="P44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="Q44" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="R44" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0</v>
       </c>
@@ -4913,16 +4925,16 @@
         <v>367</v>
       </c>
       <c r="P45" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="Q45" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="R45" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0</v>
       </c>
@@ -4969,16 +4981,16 @@
         <v>368</v>
       </c>
       <c r="P46" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="Q46" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R46" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -5025,16 +5037,16 @@
         <v>369</v>
       </c>
       <c r="P47" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q47" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="R47" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
@@ -5081,16 +5093,16 @@
         <v>370</v>
       </c>
       <c r="P48" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q48" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="R48" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -5137,16 +5149,16 @@
         <v>371</v>
       </c>
       <c r="P49" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="Q49" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="R49" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0</v>
       </c>
@@ -5193,16 +5205,16 @@
         <v>372</v>
       </c>
       <c r="P50" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q50" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="R50" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -5249,16 +5261,16 @@
         <v>373</v>
       </c>
       <c r="P51" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="Q51" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="R51" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -5305,16 +5317,16 @@
         <v>374</v>
       </c>
       <c r="P52" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="Q52" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="R52" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -5361,16 +5373,16 @@
         <v>375</v>
       </c>
       <c r="P53" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q53" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R53" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0</v>
       </c>
@@ -5417,16 +5429,16 @@
         <v>376</v>
       </c>
       <c r="P54" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="Q54" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R54" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -5473,16 +5485,16 @@
         <v>377</v>
       </c>
       <c r="P55" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q55" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R55" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0</v>
       </c>
@@ -5529,16 +5541,16 @@
         <v>378</v>
       </c>
       <c r="P56" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q56" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R56" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -5585,16 +5597,16 @@
         <v>379</v>
       </c>
       <c r="P57" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q57" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R57" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0</v>
       </c>
@@ -5641,16 +5653,16 @@
         <v>380</v>
       </c>
       <c r="P58" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q58" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="R58" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0</v>
       </c>
@@ -5697,16 +5709,16 @@
         <v>381</v>
       </c>
       <c r="P59" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q59" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R59" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -5753,16 +5765,16 @@
         <v>382</v>
       </c>
       <c r="P60" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q60" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="R60" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -5809,16 +5821,16 @@
         <v>383</v>
       </c>
       <c r="P61" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q61" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R61" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0</v>
       </c>
@@ -5865,16 +5877,16 @@
         <v>384</v>
       </c>
       <c r="P62" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q62" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R62" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0</v>
       </c>
@@ -5921,16 +5933,16 @@
         <v>385</v>
       </c>
       <c r="P63" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q63" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R63" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0</v>
       </c>
@@ -5977,16 +5989,16 @@
         <v>386</v>
       </c>
       <c r="P64" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q64" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R64" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -6033,16 +6045,16 @@
         <v>387</v>
       </c>
       <c r="P65" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="Q65" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R65" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0</v>
       </c>
@@ -6089,16 +6101,16 @@
         <v>388</v>
       </c>
       <c r="P66" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="Q66" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R66" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0</v>
       </c>
@@ -6145,16 +6157,16 @@
         <v>389</v>
       </c>
       <c r="P67" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q67" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R67" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1</v>
       </c>
@@ -6201,16 +6213,16 @@
         <v>390</v>
       </c>
       <c r="P68" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="Q68" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="R68" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0</v>
       </c>
@@ -6257,16 +6269,16 @@
         <v>391</v>
       </c>
       <c r="P69" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="Q69" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="R69" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0</v>
       </c>
@@ -6313,16 +6325,16 @@
         <v>392</v>
       </c>
       <c r="P70" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q70" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="R70" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0</v>
       </c>
@@ -6369,16 +6381,16 @@
         <v>393</v>
       </c>
       <c r="P71" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="Q71" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R71" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0</v>
       </c>
@@ -6425,16 +6437,16 @@
         <v>394</v>
       </c>
       <c r="P72" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Q72" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="R72" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0</v>
       </c>
@@ -6481,16 +6493,16 @@
         <v>395</v>
       </c>
       <c r="P73" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q73" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="R73" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -6537,16 +6549,16 @@
         <v>396</v>
       </c>
       <c r="P74" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q74" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R74" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0</v>
       </c>
@@ -6593,16 +6605,16 @@
         <v>397</v>
       </c>
       <c r="P75" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="Q75" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R75" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0</v>
       </c>
@@ -6649,16 +6661,16 @@
         <v>398</v>
       </c>
       <c r="P76" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="Q76" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R76" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1</v>
       </c>
@@ -6705,16 +6717,16 @@
         <v>399</v>
       </c>
       <c r="P77" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="Q77" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R77" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0</v>
       </c>
@@ -6761,16 +6773,16 @@
         <v>400</v>
       </c>
       <c r="P78" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="Q78" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="R78" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0</v>
       </c>
@@ -6817,16 +6829,16 @@
         <v>401</v>
       </c>
       <c r="P79" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q79" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R79" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1</v>
       </c>
@@ -6873,16 +6885,16 @@
         <v>402</v>
       </c>
       <c r="P80" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="Q80" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R80" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0</v>
       </c>
@@ -6929,16 +6941,16 @@
         <v>403</v>
       </c>
       <c r="P81" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="Q81" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="R81" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0</v>
       </c>
@@ -6985,16 +6997,16 @@
         <v>404</v>
       </c>
       <c r="P82" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="Q82" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="R82" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0</v>
       </c>
@@ -7041,16 +7053,16 @@
         <v>405</v>
       </c>
       <c r="P83" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="Q83" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="R83" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0</v>
       </c>
@@ -7097,16 +7109,16 @@
         <v>406</v>
       </c>
       <c r="P84" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Q84" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R84" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0</v>
       </c>
@@ -7153,16 +7165,16 @@
         <v>403</v>
       </c>
       <c r="P85" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Q85" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R85" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -7170,7 +7182,7 @@
         <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D86" t="s">
         <v>176</v>
@@ -7209,16 +7221,16 @@
         <v>407</v>
       </c>
       <c r="P86" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q86" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="R86" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0</v>
       </c>
@@ -7265,16 +7277,16 @@
         <v>408</v>
       </c>
       <c r="P87" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="Q87" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="R87" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1</v>
       </c>
@@ -7321,16 +7333,16 @@
         <v>409</v>
       </c>
       <c r="P88" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q88" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="R88" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0</v>
       </c>
@@ -7377,16 +7389,16 @@
         <v>410</v>
       </c>
       <c r="P89" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="Q89" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="R89" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0</v>
       </c>
@@ -7433,16 +7445,16 @@
         <v>411</v>
       </c>
       <c r="P90" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="Q90" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="R90" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0</v>
       </c>
@@ -7489,16 +7501,16 @@
         <v>412</v>
       </c>
       <c r="P91" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="Q91" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="R91" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0</v>
       </c>
@@ -7545,16 +7557,16 @@
         <v>413</v>
       </c>
       <c r="P92" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="Q92" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="R92" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0</v>
       </c>
@@ -7601,16 +7613,16 @@
         <v>414</v>
       </c>
       <c r="P93" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="Q93" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="R93" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0</v>
       </c>
@@ -7657,16 +7669,16 @@
         <v>415</v>
       </c>
       <c r="P94" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q94" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="R94" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0</v>
       </c>
@@ -7713,16 +7725,16 @@
         <v>416</v>
       </c>
       <c r="P95" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q95" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R95" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -7769,16 +7781,16 @@
         <v>417</v>
       </c>
       <c r="P96" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Q96" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="R96" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0</v>
       </c>
@@ -7825,16 +7837,16 @@
         <v>418</v>
       </c>
       <c r="P97" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q97" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="R97" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0</v>
       </c>
@@ -7881,16 +7893,16 @@
         <v>419</v>
       </c>
       <c r="P98" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Q98" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="R98" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1</v>
       </c>
@@ -7937,16 +7949,16 @@
         <v>420</v>
       </c>
       <c r="P99" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Q99" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R99" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1</v>
       </c>
@@ -7993,16 +8005,16 @@
         <v>421</v>
       </c>
       <c r="P100" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Q100" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R100" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0</v>
       </c>
@@ -8049,16 +8061,16 @@
         <v>422</v>
       </c>
       <c r="P101" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q101" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R101" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0</v>
       </c>
@@ -8105,16 +8117,16 @@
         <v>423</v>
       </c>
       <c r="P102" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q102" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R102" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1</v>
       </c>
@@ -8161,16 +8173,16 @@
         <v>124</v>
       </c>
       <c r="P103" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q103" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R103" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0</v>
       </c>
@@ -8217,16 +8229,16 @@
         <v>424</v>
       </c>
       <c r="P104" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Q104" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="R104" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0</v>
       </c>
@@ -8273,16 +8285,16 @@
         <v>425</v>
       </c>
       <c r="P105" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Q105" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="R105" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0</v>
       </c>
@@ -8329,16 +8341,16 @@
         <v>426</v>
       </c>
       <c r="P106" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="Q106" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="R106" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0</v>
       </c>
@@ -8346,7 +8358,7 @@
         <v>21</v>
       </c>
       <c r="C107" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D107" t="s">
         <v>177</v>
@@ -8385,16 +8397,16 @@
         <v>427</v>
       </c>
       <c r="P107" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q107" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="R107" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1</v>
       </c>
@@ -8441,16 +8453,16 @@
         <v>428</v>
       </c>
       <c r="P108" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="Q108" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="R108" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0</v>
       </c>
@@ -8497,16 +8509,16 @@
         <v>429</v>
       </c>
       <c r="P109" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="Q109" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R109" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0</v>
       </c>
@@ -8553,16 +8565,16 @@
         <v>430</v>
       </c>
       <c r="P110" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Q110" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="R110" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0</v>
       </c>
@@ -8609,16 +8621,16 @@
         <v>431</v>
       </c>
       <c r="P111" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q111" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="R111" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0</v>
       </c>
@@ -8665,16 +8677,16 @@
         <v>432</v>
       </c>
       <c r="P112" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q112" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="R112" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0</v>
       </c>
@@ -8721,16 +8733,16 @@
         <v>433</v>
       </c>
       <c r="P113" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="Q113" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="R113" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="114" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0</v>
       </c>
@@ -8777,16 +8789,16 @@
         <v>434</v>
       </c>
       <c r="P114" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="Q114" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="R114" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0</v>
       </c>
@@ -8833,16 +8845,16 @@
         <v>435</v>
       </c>
       <c r="P115" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="Q115" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="R115" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="116" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1</v>
       </c>
@@ -8889,16 +8901,16 @@
         <v>436</v>
       </c>
       <c r="P116" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="Q116" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="R116" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="117" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0</v>
       </c>
@@ -8945,16 +8957,16 @@
         <v>437</v>
       </c>
       <c r="P117" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Q117" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R117" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0</v>
       </c>
@@ -9001,16 +9013,16 @@
         <v>438</v>
       </c>
       <c r="P118" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="Q118" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="R118" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="119" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0</v>
       </c>
@@ -9057,16 +9069,16 @@
         <v>439</v>
       </c>
       <c r="P119" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="Q119" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="R119" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="120" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0</v>
       </c>
@@ -9113,16 +9125,16 @@
         <v>440</v>
       </c>
       <c r="P120" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Q120" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="R120" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="121" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0</v>
       </c>
@@ -9130,7 +9142,7 @@
         <v>21</v>
       </c>
       <c r="C121" t="s">
-        <v>142</v>
+        <v>667</v>
       </c>
       <c r="D121" t="s">
         <v>177</v>
@@ -9165,20 +9177,20 @@
       <c r="N121" t="s">
         <v>311</v>
       </c>
-      <c r="O121" t="s">
-        <v>441</v>
+      <c r="O121" s="1" t="s">
+        <v>669</v>
       </c>
       <c r="P121" t="s">
-        <v>469</v>
+        <v>668</v>
       </c>
       <c r="Q121" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="R121" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0</v>
       </c>
@@ -9222,19 +9234,19 @@
         <v>312</v>
       </c>
       <c r="O122" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="P122" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Q122" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R122" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="123" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0</v>
       </c>
@@ -9278,19 +9290,19 @@
         <v>313</v>
       </c>
       <c r="O123" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P123" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Q123" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R123" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0</v>
       </c>
@@ -9334,19 +9346,19 @@
         <v>314</v>
       </c>
       <c r="O124" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P124" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q124" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="R124" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="125" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0</v>
       </c>
@@ -9390,19 +9402,19 @@
         <v>312</v>
       </c>
       <c r="O125" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="P125" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q125" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="R125" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="126" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0</v>
       </c>
@@ -9446,19 +9458,19 @@
         <v>315</v>
       </c>
       <c r="O126" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P126" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q126" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="R126" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="127" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0</v>
       </c>
@@ -9505,16 +9517,16 @@
         <v>148</v>
       </c>
       <c r="P127" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q127" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R127" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="128" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0</v>
       </c>
@@ -9558,19 +9570,19 @@
         <v>317</v>
       </c>
       <c r="O128" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="P128" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="Q128" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="R128" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0</v>
       </c>
@@ -9614,19 +9626,19 @@
         <v>318</v>
       </c>
       <c r="O129" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="P129" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q129" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="R129" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>0</v>
       </c>
@@ -9670,19 +9682,19 @@
         <v>319</v>
       </c>
       <c r="O130" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P130" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="Q130" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R130" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0</v>
       </c>
@@ -9726,19 +9738,19 @@
         <v>320</v>
       </c>
       <c r="O131" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="P131" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="R131" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>0</v>
       </c>
@@ -9782,19 +9794,19 @@
         <v>321</v>
       </c>
       <c r="O132" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P132" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q132" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="R132" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>0</v>
       </c>
@@ -9838,19 +9850,19 @@
         <v>322</v>
       </c>
       <c r="O133" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P133" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="Q133" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="R133" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>0</v>
       </c>
@@ -9894,19 +9906,19 @@
         <v>323</v>
       </c>
       <c r="O134" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P134" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="Q134" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R134" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>0</v>
       </c>
@@ -9950,19 +9962,19 @@
         <v>324</v>
       </c>
       <c r="O135" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="P135" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q135" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="R135" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>0</v>
       </c>
@@ -10006,19 +10018,19 @@
         <v>325</v>
       </c>
       <c r="O136" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P136" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q136" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="R136" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>0</v>
       </c>
@@ -10062,19 +10074,19 @@
         <v>326</v>
       </c>
       <c r="O137" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P137" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Q137" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="R137" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>0</v>
       </c>
@@ -10121,16 +10133,16 @@
         <v>159</v>
       </c>
       <c r="P138" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q138" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R138" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>0</v>
       </c>
@@ -10177,16 +10189,16 @@
         <v>160</v>
       </c>
       <c r="P139" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q139" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R139" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>0</v>
       </c>
@@ -10230,19 +10242,19 @@
         <v>329</v>
       </c>
       <c r="O140" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="P140" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q140" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="R140" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>0</v>
       </c>
@@ -10286,19 +10298,19 @@
         <v>330</v>
       </c>
       <c r="O141" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="P141" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="Q141" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="R141" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>0</v>
       </c>
@@ -10342,19 +10354,19 @@
         <v>331</v>
       </c>
       <c r="O142" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P142" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="Q142" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="R142" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1</v>
       </c>
@@ -10398,19 +10410,19 @@
         <v>332</v>
       </c>
       <c r="O143" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P143" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="Q143" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R143" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>0</v>
       </c>
@@ -10454,19 +10466,19 @@
         <v>333</v>
       </c>
       <c r="O144" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P144" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q144" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="R144" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="145" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>0</v>
       </c>
@@ -10510,19 +10522,19 @@
         <v>334</v>
       </c>
       <c r="O145" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P145" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="Q145" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="R145" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="146" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>0</v>
       </c>
@@ -10566,19 +10578,19 @@
         <v>322</v>
       </c>
       <c r="O146" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="P146" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="Q146" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="R146" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="147" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>0</v>
       </c>
@@ -10622,19 +10634,19 @@
         <v>335</v>
       </c>
       <c r="O147" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P147" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q147" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="R147" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="148" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1</v>
       </c>
@@ -10678,19 +10690,19 @@
         <v>336</v>
       </c>
       <c r="O148" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P148" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="Q148" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="R148" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>0</v>
       </c>
@@ -10734,19 +10746,19 @@
         <v>332</v>
       </c>
       <c r="O149" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P149" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q149" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="R149" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="150" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>0</v>
       </c>
@@ -10790,19 +10802,19 @@
         <v>337</v>
       </c>
       <c r="O150" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P150" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="Q150" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R150" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="151" spans="1:18">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>0</v>
       </c>
@@ -10846,16 +10858,16 @@
         <v>323</v>
       </c>
       <c r="O151" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P151" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Q151" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="R151" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>